<commit_message>
ADD Excel File linking issue solved
</commit_message>
<xml_diff>
--- a/scripts/Num_of_rating_per_Gender_Age_Genre.xlsx
+++ b/scripts/Num_of_rating_per_Gender_Age_Genre.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujinlee/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720B569B-D4EA-F140-84FB-D13C0D4AE801}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54269B5D-EAA5-904B-968F-145F42188D48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="3260" windowWidth="27240" windowHeight="16440" xr2:uid="{B18A1EE7-9501-C74B-92F1-3A541601984D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -230,26 +227,7 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF9C5700"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -260,35 +238,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98677C87-2A2B-2743-8830-50C0707936DE}" name="Table4" displayName="Table4" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Neutral">
-  <autoFilter ref="A1:D1048576" xr:uid="{74896DA6-B8DA-5B4D-822F-C54710EDD4C9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D1048576">
-    <sortCondition ref="D1:D1048576"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{55FA6033-0175-8145-9DA6-72CE091C8D1A}" name="Gender"/>
-    <tableColumn id="2" xr3:uid="{51102032-3239-4842-9CA7-294B67421F09}" name="Age"/>
-    <tableColumn id="3" xr3:uid="{C2DE35A1-8B69-764A-ACDD-D1E016BA5D84}" name="Genre"/>
-    <tableColumn id="4" xr3:uid="{CAA69056-AD51-F246-8F9F-4EF52FE37483}" name="Num of R"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,12 +540,12 @@
   <dimension ref="A1:D253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -620,11 +569,10 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2">
-        <f>COUNTIFS([1]!Table3[Gender],A2,[1]!Table3[Age],B2,[1]!Table3[Documentary],1)</f>
         <v>25</v>
       </c>
     </row>
@@ -635,11 +583,10 @@
       <c r="B3">
         <v>56</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3">
-        <f>COUNTIFS([1]!Table3[Gender],A3,[1]!Table3[Age],B3,[1]!Table3[Documentary],1)</f>
         <v>72</v>
       </c>
     </row>
@@ -650,26 +597,24 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4">
-        <f>COUNTIFS([1]!Table3[Gender],A4,[1]!Table3[Age],B4,[1]!Table3[Film-Noir],1)</f>
         <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5">
-        <f>COUNTIFS([1]!Table3[Gender],A5,[1]!Table3[Age],B5,[1]!Table3[Western],1)</f>
         <v>91</v>
       </c>
     </row>
@@ -680,11 +625,10 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6">
-        <f>COUNTIFS([1]!Table3[Gender],A6,[1]!Table3[Age],B6,[1]!Table3[Documentary],1)</f>
         <v>105</v>
       </c>
     </row>
@@ -695,11 +639,10 @@
       <c r="B7">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7">
-        <f>COUNTIFS([1]!Table3[Gender],A7,[1]!Table3[Age],B7,[1]!Table3[Documentary],1)</f>
         <v>167</v>
       </c>
     </row>
@@ -710,11 +653,10 @@
       <c r="B8">
         <v>56</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8">
-        <f>COUNTIFS([1]!Table3[Gender],A8,[1]!Table3[Age],B8,[1]!Table3[Documentary],1)</f>
         <v>188</v>
       </c>
     </row>
@@ -725,11 +667,10 @@
       <c r="B9">
         <v>56</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9">
-        <f>COUNTIFS([1]!Table3[Gender],A9,[1]!Table3[Age],B9,[1]!Table3[Fantasy],1)</f>
         <v>191</v>
       </c>
     </row>
@@ -740,26 +681,24 @@
       <c r="B10">
         <v>45</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10">
-        <f>COUNTIFS([1]!Table3[Gender],A10,[1]!Table3[Age],B10,[1]!Table3[Documentary],1)</f>
         <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
         <v>56</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
       <c r="D11">
-        <f>COUNTIFS([1]!Table3[Gender],A11,[1]!Table3[Age],B11,[1]!Table3[Western],1)</f>
         <v>220</v>
       </c>
     </row>
@@ -770,41 +709,38 @@
       <c r="B12">
         <v>18</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="D12">
-        <f>COUNTIFS([1]!Table3[Gender],A12,[1]!Table3[Age],B12,[1]!Table3[Documentary],1)</f>
         <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13">
-        <f>COUNTIFS([1]!Table3[Gender],A13,[1]!Table3[Age],B13,[1]!Table3[Western],1)</f>
         <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14">
-        <f>COUNTIFS([1]!Table3[Gender],A14,[1]!Table3[Age],B14,[1]!Table3[Mystery],1)</f>
         <v>246</v>
       </c>
     </row>
@@ -815,11 +751,10 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
       <c r="D15">
-        <f>COUNTIFS([1]!Table3[Gender],A15,[1]!Table3[Age],B15,[1]!Table3[Film-Noir],1)</f>
         <v>250</v>
       </c>
     </row>
@@ -830,11 +765,10 @@
       <c r="B16">
         <v>56</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16">
-        <f>COUNTIFS([1]!Table3[Gender],A16,[1]!Table3[Age],B16,[1]!Table3[Film-Noir],1)</f>
         <v>306</v>
       </c>
     </row>
@@ -849,7 +783,6 @@
         <v>8</v>
       </c>
       <c r="D17">
-        <f>COUNTIFS([1]!Table3[Gender],A17,[1]!Table3[Age],B17,[1]!Table3[Animation],1)</f>
         <v>313</v>
       </c>
     </row>
@@ -860,26 +793,24 @@
       <c r="B18">
         <v>56</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18">
-        <f>COUNTIFS([1]!Table3[Gender],A18,[1]!Table3[Age],B18,[1]!Table3[Horror],1)</f>
         <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
         <v>50</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>23</v>
       </c>
       <c r="D19">
-        <f>COUNTIFS([1]!Table3[Gender],A19,[1]!Table3[Age],B19,[1]!Table3[Western],1)</f>
         <v>330</v>
       </c>
     </row>
@@ -890,26 +821,24 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20">
-        <f>COUNTIFS([1]!Table3[Gender],A20,[1]!Table3[Age],B20,[1]!Table3[Crime],1)</f>
         <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>22</v>
       </c>
       <c r="D21">
-        <f>COUNTIFS([1]!Table3[Gender],A21,[1]!Table3[Age],B21,[1]!Table3[War],1)</f>
         <v>374</v>
       </c>
     </row>
@@ -920,11 +849,10 @@
       <c r="B22">
         <v>50</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22">
-        <f>COUNTIFS([1]!Table3[Gender],A22,[1]!Table3[Age],B22,[1]!Table3[Documentary],1)</f>
         <v>388</v>
       </c>
     </row>
@@ -935,11 +863,10 @@
       <c r="B23">
         <v>35</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23">
-        <f>COUNTIFS([1]!Table3[Gender],A23,[1]!Table3[Age],B23,[1]!Table3[Documentary],1)</f>
         <v>419</v>
       </c>
     </row>
@@ -950,11 +877,10 @@
       <c r="B24">
         <v>50</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24">
-        <f>COUNTIFS([1]!Table3[Gender],A24,[1]!Table3[Age],B24,[1]!Table3[Film-Noir],1)</f>
         <v>467</v>
       </c>
     </row>
@@ -965,11 +891,10 @@
       <c r="B25">
         <v>18</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>15</v>
       </c>
       <c r="D25">
-        <f>COUNTIFS([1]!Table3[Gender],A25,[1]!Table3[Age],B25,[1]!Table3[Film-Noir],1)</f>
         <v>474</v>
       </c>
     </row>
@@ -980,11 +905,10 @@
       <c r="B26">
         <v>45</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26">
-        <f>COUNTIFS([1]!Table3[Gender],A26,[1]!Table3[Age],B26,[1]!Table3[Documentary],1)</f>
         <v>484</v>
       </c>
     </row>
@@ -995,11 +919,10 @@
       <c r="B27">
         <v>45</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="s">
         <v>15</v>
       </c>
       <c r="D27">
-        <f>COUNTIFS([1]!Table3[Gender],A27,[1]!Table3[Age],B27,[1]!Table3[Film-Noir],1)</f>
         <v>489</v>
       </c>
     </row>
@@ -1010,11 +933,10 @@
       <c r="B28">
         <v>50</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28">
-        <f>COUNTIFS([1]!Table3[Gender],A28,[1]!Table3[Age],B28,[1]!Table3[Fantasy],1)</f>
         <v>492</v>
       </c>
     </row>
@@ -1029,52 +951,48 @@
         <v>9</v>
       </c>
       <c r="D29">
-        <f>COUNTIFS([1]!Table3[Gender],A29,[1]!Table3[Age],B29,[1]!Table3[Children''s],1)</f>
         <v>496</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="3">
-        <v>18</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30">
-        <f>COUNTIFS([1]!Table3[Gender],A30,[1]!Table3[Age],B30,[1]!Table3[Western],1)</f>
         <v>503</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="3">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
         <v>56</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" t="s">
         <v>18</v>
       </c>
       <c r="D31">
-        <f>COUNTIFS([1]!Table3[Gender],A31,[1]!Table3[Age],B31,[1]!Table3[Mystery],1)</f>
         <v>506</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="3">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
         <v>45</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32">
-        <f>COUNTIFS([1]!Table3[Gender],A32,[1]!Table3[Age],B32,[1]!Table3[Western],1)</f>
         <v>508</v>
       </c>
     </row>
@@ -1085,11 +1003,10 @@
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" t="s">
         <v>14</v>
       </c>
       <c r="D33">
-        <f>COUNTIFS([1]!Table3[Gender],A33,[1]!Table3[Age],B33,[1]!Table3[Fantasy],1)</f>
         <v>523</v>
       </c>
     </row>
@@ -1100,26 +1017,24 @@
       <c r="B34">
         <v>56</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" t="s">
         <v>11</v>
       </c>
       <c r="D34">
-        <f>COUNTIFS([1]!Table3[Gender],A34,[1]!Table3[Age],B34,[1]!Table3[Crime],1)</f>
         <v>581</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="3">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
         <v>56</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" t="s">
         <v>17</v>
       </c>
       <c r="D35">
-        <f>COUNTIFS([1]!Table3[Gender],A35,[1]!Table3[Age],B35,[1]!Table3[Musical],1)</f>
         <v>599</v>
       </c>
     </row>
@@ -1134,7 +1049,6 @@
         <v>8</v>
       </c>
       <c r="D36">
-        <f>COUNTIFS([1]!Table3[Gender],A36,[1]!Table3[Age],B36,[1]!Table3[Animation],1)</f>
         <v>621</v>
       </c>
     </row>
@@ -1145,26 +1059,24 @@
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" t="s">
         <v>16</v>
       </c>
       <c r="D37">
-        <f>COUNTIFS([1]!Table3[Gender],A37,[1]!Table3[Age],B37,[1]!Table3[Horror],1)</f>
         <v>640</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="3">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" t="s">
         <v>18</v>
       </c>
       <c r="D38">
-        <f>COUNTIFS([1]!Table3[Gender],A38,[1]!Table3[Age],B38,[1]!Table3[Mystery],1)</f>
         <v>674</v>
       </c>
     </row>
@@ -1175,11 +1087,10 @@
       <c r="B39">
         <v>50</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
         <v>16</v>
       </c>
       <c r="D39">
-        <f>COUNTIFS([1]!Table3[Gender],A39,[1]!Table3[Age],B39,[1]!Table3[Horror],1)</f>
         <v>728</v>
       </c>
     </row>
@@ -1190,11 +1101,10 @@
       <c r="B40">
         <v>56</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40">
-        <f>COUNTIFS([1]!Table3[Gender],A40,[1]!Table3[Age],B40,[1]!Table3[Fantasy],1)</f>
         <v>757</v>
       </c>
     </row>
@@ -1209,7 +1119,6 @@
         <v>8</v>
       </c>
       <c r="D41">
-        <f>COUNTIFS([1]!Table3[Gender],A41,[1]!Table3[Age],B41,[1]!Table3[Animation],1)</f>
         <v>770</v>
       </c>
     </row>
@@ -1220,56 +1129,52 @@
       <c r="B42">
         <v>45</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42">
-        <f>COUNTIFS([1]!Table3[Gender],A42,[1]!Table3[Age],B42,[1]!Table3[Fantasy],1)</f>
         <v>782</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="3">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
         <v>35</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" t="s">
         <v>23</v>
       </c>
       <c r="D43">
-        <f>COUNTIFS([1]!Table3[Gender],A43,[1]!Table3[Age],B43,[1]!Table3[Western],1)</f>
         <v>791</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="3">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44">
         <v>56</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" t="s">
         <v>22</v>
       </c>
       <c r="D44">
-        <f>COUNTIFS([1]!Table3[Gender],A44,[1]!Table3[Age],B44,[1]!Table3[War],1)</f>
         <v>802</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="3">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45">
         <v>56</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" t="s">
         <v>20</v>
       </c>
       <c r="D45">
-        <f>COUNTIFS([1]!Table3[Gender],A45,[1]!Table3[Age],B45,[1]!Table3[Sci-Fi],1)</f>
         <v>807</v>
       </c>
     </row>
@@ -1284,22 +1189,20 @@
         <v>7</v>
       </c>
       <c r="D46">
-        <f>COUNTIFS([1]!Table3[Gender],A46,[1]!Table3[Age],B46,[1]!Table3[Adventure],1)</f>
         <v>808</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="3">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47">
         <v>1</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" t="s">
         <v>17</v>
       </c>
       <c r="D47">
-        <f>COUNTIFS([1]!Table3[Gender],A47,[1]!Table3[Age],B47,[1]!Table3[Musical],1)</f>
         <v>817</v>
       </c>
     </row>
@@ -1310,26 +1213,24 @@
       <c r="B48">
         <v>25</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" t="s">
         <v>12</v>
       </c>
       <c r="D48">
-        <f>COUNTIFS([1]!Table3[Gender],A48,[1]!Table3[Age],B48,[1]!Table3[Documentary],1)</f>
         <v>819</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="3">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" t="s">
         <v>17</v>
       </c>
       <c r="D49">
-        <f>COUNTIFS([1]!Table3[Gender],A49,[1]!Table3[Age],B49,[1]!Table3[Musical],1)</f>
         <v>830</v>
       </c>
     </row>
@@ -1340,11 +1241,10 @@
       <c r="B50">
         <v>1</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" t="s">
         <v>14</v>
       </c>
       <c r="D50">
-        <f>COUNTIFS([1]!Table3[Gender],A50,[1]!Table3[Age],B50,[1]!Table3[Fantasy],1)</f>
         <v>837</v>
       </c>
     </row>
@@ -1355,11 +1255,10 @@
       <c r="B51">
         <v>18</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" t="s">
         <v>12</v>
       </c>
       <c r="D51">
-        <f>COUNTIFS([1]!Table3[Gender],A51,[1]!Table3[Age],B51,[1]!Table3[Documentary],1)</f>
         <v>846</v>
       </c>
     </row>
@@ -1370,11 +1269,10 @@
       <c r="B52">
         <v>56</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52">
-        <f>COUNTIFS([1]!Table3[Gender],A52,[1]!Table3[Age],B52,[1]!Table3[Film-Noir],1)</f>
         <v>901</v>
       </c>
     </row>
@@ -1389,52 +1287,48 @@
         <v>8</v>
       </c>
       <c r="D53">
-        <f>COUNTIFS([1]!Table3[Gender],A53,[1]!Table3[Age],B53,[1]!Table3[Animation],1)</f>
         <v>922</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="3">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54">
         <v>1</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" t="s">
         <v>20</v>
       </c>
       <c r="D54">
-        <f>COUNTIFS([1]!Table3[Gender],A54,[1]!Table3[Age],B54,[1]!Table3[Sci-Fi],1)</f>
         <v>946</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="3">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55">
         <v>50</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" t="s">
         <v>18</v>
       </c>
       <c r="D55">
-        <f>COUNTIFS([1]!Table3[Gender],A55,[1]!Table3[Age],B55,[1]!Table3[Mystery],1)</f>
         <v>947</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="3">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56">
         <v>50</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" t="s">
         <v>17</v>
       </c>
       <c r="D56">
-        <f>COUNTIFS([1]!Table3[Gender],A56,[1]!Table3[Age],B56,[1]!Table3[Musical],1)</f>
         <v>973</v>
       </c>
     </row>
@@ -1449,7 +1343,6 @@
         <v>8</v>
       </c>
       <c r="D57">
-        <f>COUNTIFS([1]!Table3[Gender],A57,[1]!Table3[Age],B57,[1]!Table3[Animation],1)</f>
         <v>1010</v>
       </c>
     </row>
@@ -1464,67 +1357,62 @@
         <v>15</v>
       </c>
       <c r="D58">
-        <f>COUNTIFS([1]!Table3[Gender],A58,[1]!Table3[Age],B58,[1]!Table3[Film-Noir],1)</f>
         <v>1012</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="3">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59">
         <v>25</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D59">
-        <f>COUNTIFS([1]!Table3[Gender],A59,[1]!Table3[Age],B59,[1]!Table3[Western],1)</f>
         <v>1034</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60" s="3">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D60">
-        <f>COUNTIFS([1]!Table3[Gender],A60,[1]!Table3[Age],B60,[1]!Table3[Thriller],1)</f>
         <v>1112</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="3">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61">
         <v>56</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D61">
-        <f>COUNTIFS([1]!Table3[Gender],A61,[1]!Table3[Age],B61,[1]!Table3[Western],1)</f>
         <v>1113</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" s="3">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62">
         <v>45</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D62">
-        <f>COUNTIFS([1]!Table3[Gender],A62,[1]!Table3[Age],B62,[1]!Table3[Mystery],1)</f>
         <v>1133</v>
       </c>
     </row>
@@ -1535,26 +1423,24 @@
       <c r="B63">
         <v>50</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D63">
-        <f>COUNTIFS([1]!Table3[Gender],A63,[1]!Table3[Age],B63,[1]!Table3[Children''s],1)</f>
         <v>1137</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B64" s="3">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D64">
-        <f>COUNTIFS([1]!Table3[Gender],A64,[1]!Table3[Age],B64,[1]!Table3[War],1)</f>
         <v>1204</v>
       </c>
     </row>
@@ -1565,26 +1451,24 @@
       <c r="B65">
         <v>1</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D65">
-        <f>COUNTIFS([1]!Table3[Gender],A65,[1]!Table3[Age],B65,[1]!Table3[Adventure],1)</f>
         <v>1230</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B66" s="3">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66">
         <v>56</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D66">
-        <f>COUNTIFS([1]!Table3[Gender],A66,[1]!Table3[Age],B66,[1]!Table3[Thriller],1)</f>
         <v>1246</v>
       </c>
     </row>
@@ -1595,26 +1479,24 @@
       <c r="B67">
         <v>56</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D67">
-        <f>COUNTIFS([1]!Table3[Gender],A67,[1]!Table3[Age],B67,[1]!Table3[Action],1)</f>
         <v>1260</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B68" s="3">
+      <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68">
         <v>50</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D68">
-        <f>COUNTIFS([1]!Table3[Gender],A68,[1]!Table3[Age],B68,[1]!Table3[War],1)</f>
         <v>1280</v>
       </c>
     </row>
@@ -1629,7 +1511,6 @@
         <v>11</v>
       </c>
       <c r="D69">
-        <f>COUNTIFS([1]!Table3[Gender],A69,[1]!Table3[Age],B69,[1]!Table3[Crime],1)</f>
         <v>1285</v>
       </c>
     </row>
@@ -1644,22 +1525,20 @@
         <v>12</v>
       </c>
       <c r="D70">
-        <f>COUNTIFS([1]!Table3[Gender],A70,[1]!Table3[Age],B70,[1]!Table3[Documentary],1)</f>
         <v>1289</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B71" s="3">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71">
         <v>56</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D71">
-        <f>COUNTIFS([1]!Table3[Gender],A71,[1]!Table3[Age],B71,[1]!Table3[Musical],1)</f>
         <v>1290</v>
       </c>
     </row>
@@ -1674,7 +1553,6 @@
         <v>16</v>
       </c>
       <c r="D72">
-        <f>COUNTIFS([1]!Table3[Gender],A72,[1]!Table3[Age],B72,[1]!Table3[Horror],1)</f>
         <v>1319</v>
       </c>
     </row>
@@ -1689,7 +1567,6 @@
         <v>11</v>
       </c>
       <c r="D73">
-        <f>COUNTIFS([1]!Table3[Gender],A73,[1]!Table3[Age],B73,[1]!Table3[Crime],1)</f>
         <v>1336</v>
       </c>
     </row>
@@ -1700,11 +1577,10 @@
       <c r="B74">
         <v>1</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D74">
-        <f>COUNTIFS([1]!Table3[Gender],A74,[1]!Table3[Age],B74,[1]!Table3[Action],1)</f>
         <v>1343</v>
       </c>
     </row>
@@ -1719,7 +1595,6 @@
         <v>15</v>
       </c>
       <c r="D75">
-        <f>COUNTIFS([1]!Table3[Gender],A75,[1]!Table3[Age],B75,[1]!Table3[Film-Noir],1)</f>
         <v>1371</v>
       </c>
     </row>
@@ -1734,7 +1609,6 @@
         <v>15</v>
       </c>
       <c r="D76">
-        <f>COUNTIFS([1]!Table3[Gender],A76,[1]!Table3[Age],B76,[1]!Table3[Film-Noir],1)</f>
         <v>1374</v>
       </c>
     </row>
@@ -1745,11 +1619,10 @@
       <c r="B77">
         <v>56</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D77">
-        <f>COUNTIFS([1]!Table3[Gender],A77,[1]!Table3[Age],B77,[1]!Table3[Children''s],1)</f>
         <v>1392</v>
       </c>
     </row>
@@ -1764,7 +1637,6 @@
         <v>15</v>
       </c>
       <c r="D78">
-        <f>COUNTIFS([1]!Table3[Gender],A78,[1]!Table3[Age],B78,[1]!Table3[Film-Noir],1)</f>
         <v>1403</v>
       </c>
     </row>
@@ -1775,26 +1647,24 @@
       <c r="B79">
         <v>50</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D79">
-        <f>COUNTIFS([1]!Table3[Gender],A79,[1]!Table3[Age],B79,[1]!Table3[Animation],1)</f>
         <v>1411</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="3">
+      <c r="A80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80">
         <v>45</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D80">
-        <f>COUNTIFS([1]!Table3[Gender],A80,[1]!Table3[Age],B80,[1]!Table3[Musical],1)</f>
         <v>1413</v>
       </c>
     </row>
@@ -1809,7 +1679,6 @@
         <v>16</v>
       </c>
       <c r="D81">
-        <f>COUNTIFS([1]!Table3[Gender],A81,[1]!Table3[Age],B81,[1]!Table3[Horror],1)</f>
         <v>1436</v>
       </c>
     </row>
@@ -1820,26 +1689,24 @@
       <c r="B82">
         <v>1</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D82">
-        <f>COUNTIFS([1]!Table3[Gender],A82,[1]!Table3[Age],B82,[1]!Table3[Animation],1)</f>
         <v>1439</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B83" s="3">
+      <c r="A83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83">
         <v>18</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D83">
-        <f>COUNTIFS([1]!Table3[Gender],A83,[1]!Table3[Age],B83,[1]!Table3[Mystery],1)</f>
         <v>1467</v>
       </c>
     </row>
@@ -1854,7 +1721,6 @@
         <v>16</v>
       </c>
       <c r="D84">
-        <f>COUNTIFS([1]!Table3[Gender],A84,[1]!Table3[Age],B84,[1]!Table3[Horror],1)</f>
         <v>1571</v>
       </c>
     </row>
@@ -1869,22 +1735,20 @@
         <v>11</v>
       </c>
       <c r="D85">
-        <f>COUNTIFS([1]!Table3[Gender],A85,[1]!Table3[Age],B85,[1]!Table3[Crime],1)</f>
         <v>1601</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B86" s="3">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86">
         <v>45</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D86">
-        <f>COUNTIFS([1]!Table3[Gender],A86,[1]!Table3[Age],B86,[1]!Table3[Western],1)</f>
         <v>1625</v>
       </c>
     </row>
@@ -1899,52 +1763,48 @@
         <v>14</v>
       </c>
       <c r="D87">
-        <f>COUNTIFS([1]!Table3[Gender],A87,[1]!Table3[Age],B87,[1]!Table3[Fantasy],1)</f>
         <v>1635</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B88" s="3">
+      <c r="A88" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88">
         <v>1</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D88">
-        <f>COUNTIFS([1]!Table3[Gender],A88,[1]!Table3[Age],B88,[1]!Table3[Romance],1)</f>
         <v>1637</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B89" s="3">
+      <c r="A89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89">
         <v>56</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D89">
-        <f>COUNTIFS([1]!Table3[Gender],A89,[1]!Table3[Age],B89,[1]!Table3[Mystery],1)</f>
         <v>1641</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B90" s="3">
+      <c r="A90" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90">
         <v>45</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D90">
-        <f>COUNTIFS([1]!Table3[Gender],A90,[1]!Table3[Age],B90,[1]!Table3[War],1)</f>
         <v>1675</v>
       </c>
     </row>
@@ -1955,11 +1815,10 @@
       <c r="B91">
         <v>45</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D91">
-        <f>COUNTIFS([1]!Table3[Gender],A91,[1]!Table3[Age],B91,[1]!Table3[Children''s],1)</f>
         <v>1704</v>
       </c>
     </row>
@@ -1970,11 +1829,10 @@
       <c r="B92">
         <v>50</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D92">
-        <f>COUNTIFS([1]!Table3[Gender],A92,[1]!Table3[Age],B92,[1]!Table3[Adventure],1)</f>
         <v>1754</v>
       </c>
     </row>
@@ -1989,7 +1847,6 @@
         <v>14</v>
       </c>
       <c r="D93">
-        <f>COUNTIFS([1]!Table3[Gender],A93,[1]!Table3[Age],B93,[1]!Table3[Fantasy],1)</f>
         <v>1772</v>
       </c>
     </row>
@@ -2004,22 +1861,20 @@
         <v>15</v>
       </c>
       <c r="D94">
-        <f>COUNTIFS([1]!Table3[Gender],A94,[1]!Table3[Age],B94,[1]!Table3[Film-Noir],1)</f>
         <v>1806</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B95" s="3">
+      <c r="A95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95">
         <v>50</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D95">
-        <f>COUNTIFS([1]!Table3[Gender],A95,[1]!Table3[Age],B95,[1]!Table3[Sci-Fi],1)</f>
         <v>1806</v>
       </c>
     </row>
@@ -2034,7 +1889,6 @@
         <v>14</v>
       </c>
       <c r="D96">
-        <f>COUNTIFS([1]!Table3[Gender],A96,[1]!Table3[Age],B96,[1]!Table3[Fantasy],1)</f>
         <v>1913</v>
       </c>
     </row>
@@ -2049,22 +1903,20 @@
         <v>14</v>
       </c>
       <c r="D97">
-        <f>COUNTIFS([1]!Table3[Gender],A97,[1]!Table3[Age],B97,[1]!Table3[Fantasy],1)</f>
         <v>1934</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B98" s="3">
+      <c r="A98" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98">
         <v>1</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D98">
-        <f>COUNTIFS([1]!Table3[Gender],A98,[1]!Table3[Age],B98,[1]!Table3[Romance],1)</f>
         <v>1962</v>
       </c>
     </row>
@@ -2075,11 +1927,10 @@
       <c r="B99">
         <v>45</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D99">
-        <f>COUNTIFS([1]!Table3[Gender],A99,[1]!Table3[Age],B99,[1]!Table3[Animation],1)</f>
         <v>1967</v>
       </c>
     </row>
@@ -2090,86 +1941,80 @@
       <c r="B100">
         <v>1</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D100">
-        <f>COUNTIFS([1]!Table3[Gender],A100,[1]!Table3[Age],B100,[1]!Table3[Children''s],1)</f>
         <v>2024</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B101" s="3">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101">
         <v>56</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D101">
-        <f>COUNTIFS([1]!Table3[Gender],A101,[1]!Table3[Age],B101,[1]!Table3[Romance],1)</f>
         <v>2031</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B102" s="3">
+      <c r="A102" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102">
         <v>50</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D102">
-        <f>COUNTIFS([1]!Table3[Gender],A102,[1]!Table3[Age],B102,[1]!Table3[Western],1)</f>
         <v>2090</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B103" s="3">
+      <c r="A103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103">
         <v>50</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D103">
-        <f>COUNTIFS([1]!Table3[Gender],A103,[1]!Table3[Age],B103,[1]!Table3[Musical],1)</f>
         <v>2120</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B104" s="3">
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104">
         <v>35</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D104">
-        <f>COUNTIFS([1]!Table3[Gender],A104,[1]!Table3[Age],B104,[1]!Table3[Mystery],1)</f>
         <v>2192</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B105" s="3">
+      <c r="A105" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105">
         <v>18</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D105">
-        <f>COUNTIFS([1]!Table3[Gender],A105,[1]!Table3[Age],B105,[1]!Table3[War],1)</f>
         <v>2204</v>
       </c>
     </row>
@@ -2180,26 +2025,24 @@
       <c r="B106">
         <v>1</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D106">
-        <f>COUNTIFS([1]!Table3[Gender],A106,[1]!Table3[Age],B106,[1]!Table3[Children''s],1)</f>
         <v>2313</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B107" s="3">
+      <c r="A107" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107">
         <v>18</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D107">
-        <f>COUNTIFS([1]!Table3[Gender],A107,[1]!Table3[Age],B107,[1]!Table3[Western],1)</f>
         <v>2360</v>
       </c>
     </row>
@@ -2214,7 +2057,6 @@
         <v>11</v>
       </c>
       <c r="D108">
-        <f>COUNTIFS([1]!Table3[Gender],A108,[1]!Table3[Age],B108,[1]!Table3[Crime],1)</f>
         <v>2393</v>
       </c>
     </row>
@@ -2225,41 +2067,38 @@
       <c r="B109">
         <v>35</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D109">
-        <f>COUNTIFS([1]!Table3[Gender],A109,[1]!Table3[Age],B109,[1]!Table3[Animation],1)</f>
         <v>2399</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B110" s="3">
+      <c r="A110" t="s">
+        <v>6</v>
+      </c>
+      <c r="B110">
         <v>45</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D110">
-        <f>COUNTIFS([1]!Table3[Gender],A110,[1]!Table3[Age],B110,[1]!Table3[Musical],1)</f>
         <v>2485</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B111" s="3">
+      <c r="A111" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111">
         <v>50</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D111">
-        <f>COUNTIFS([1]!Table3[Gender],A111,[1]!Table3[Age],B111,[1]!Table3[Mystery],1)</f>
         <v>2573</v>
       </c>
     </row>
@@ -2270,26 +2109,24 @@
       <c r="B112">
         <v>45</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D112">
-        <f>COUNTIFS([1]!Table3[Gender],A112,[1]!Table3[Age],B112,[1]!Table3[Adventure],1)</f>
         <v>2648</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B113" s="3">
+      <c r="A113" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113">
         <v>35</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D113">
-        <f>COUNTIFS([1]!Table3[Gender],A113,[1]!Table3[Age],B113,[1]!Table3[Musical],1)</f>
         <v>2668</v>
       </c>
     </row>
@@ -2304,7 +2141,6 @@
         <v>12</v>
       </c>
       <c r="D114">
-        <f>COUNTIFS([1]!Table3[Gender],A114,[1]!Table3[Age],B114,[1]!Table3[Documentary],1)</f>
         <v>2670</v>
       </c>
     </row>
@@ -2319,37 +2155,34 @@
         <v>13</v>
       </c>
       <c r="D115">
-        <f>COUNTIFS([1]!Table3[Gender],A115,[1]!Table3[Age],B115,[1]!Table3[Drama],1)</f>
         <v>2671</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B116" s="3">
+      <c r="A116" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116">
         <v>45</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D116">
-        <f>COUNTIFS([1]!Table3[Gender],A116,[1]!Table3[Age],B116,[1]!Table3[Mystery],1)</f>
         <v>2718</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B117" s="3">
+      <c r="A117" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117">
         <v>18</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D117">
-        <f>COUNTIFS([1]!Table3[Gender],A117,[1]!Table3[Age],B117,[1]!Table3[Musical],1)</f>
         <v>2735</v>
       </c>
     </row>
@@ -2360,11 +2193,10 @@
       <c r="B118">
         <v>50</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D118">
-        <f>COUNTIFS([1]!Table3[Gender],A118,[1]!Table3[Age],B118,[1]!Table3[Children''s],1)</f>
         <v>2753</v>
       </c>
     </row>
@@ -2375,26 +2207,24 @@
       <c r="B119">
         <v>1</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D119">
-        <f>COUNTIFS([1]!Table3[Gender],A119,[1]!Table3[Age],B119,[1]!Table3[Adventure],1)</f>
         <v>2768</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B120" s="3">
+      <c r="A120" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120">
         <v>45</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D120">
-        <f>COUNTIFS([1]!Table3[Gender],A120,[1]!Table3[Age],B120,[1]!Table3[Sci-Fi],1)</f>
         <v>2787</v>
       </c>
     </row>
@@ -2409,37 +2239,34 @@
         <v>11</v>
       </c>
       <c r="D121">
-        <f>COUNTIFS([1]!Table3[Gender],A121,[1]!Table3[Age],B121,[1]!Table3[Crime],1)</f>
         <v>2875</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B122" s="3">
+      <c r="A122" t="s">
+        <v>4</v>
+      </c>
+      <c r="B122">
         <v>50</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D122">
-        <f>COUNTIFS([1]!Table3[Gender],A122,[1]!Table3[Age],B122,[1]!Table3[Thriller],1)</f>
         <v>2886</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B123" s="3">
+      <c r="A123" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123">
         <v>56</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D123">
-        <f>COUNTIFS([1]!Table3[Gender],A123,[1]!Table3[Age],B123,[1]!Table3[War],1)</f>
         <v>2973</v>
       </c>
     </row>
@@ -2454,7 +2281,6 @@
         <v>10</v>
       </c>
       <c r="D124">
-        <f>COUNTIFS([1]!Table3[Gender],A124,[1]!Table3[Age],B124,[1]!Table3[Comedy],1)</f>
         <v>2978</v>
       </c>
     </row>
@@ -2465,11 +2291,10 @@
       <c r="B125">
         <v>50</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D125">
-        <f>COUNTIFS([1]!Table3[Gender],A125,[1]!Table3[Age],B125,[1]!Table3[Action],1)</f>
         <v>2993</v>
       </c>
     </row>
@@ -2484,7 +2309,6 @@
         <v>14</v>
       </c>
       <c r="D126">
-        <f>COUNTIFS([1]!Table3[Gender],A126,[1]!Table3[Age],B126,[1]!Table3[Fantasy],1)</f>
         <v>3024</v>
       </c>
     </row>
@@ -2499,22 +2323,20 @@
         <v>16</v>
       </c>
       <c r="D127">
-        <f>COUNTIFS([1]!Table3[Gender],A127,[1]!Table3[Age],B127,[1]!Table3[Horror],1)</f>
         <v>3081</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B128" s="3">
+      <c r="A128" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128">
         <v>35</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D128">
-        <f>COUNTIFS([1]!Table3[Gender],A128,[1]!Table3[Age],B128,[1]!Table3[War],1)</f>
         <v>3097</v>
       </c>
     </row>
@@ -2525,11 +2347,10 @@
       <c r="B129">
         <v>18</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D129">
-        <f>COUNTIFS([1]!Table3[Gender],A129,[1]!Table3[Age],B129,[1]!Table3[Animation],1)</f>
         <v>3109</v>
       </c>
     </row>
@@ -2544,7 +2365,6 @@
         <v>15</v>
       </c>
       <c r="D130">
-        <f>COUNTIFS([1]!Table3[Gender],A130,[1]!Table3[Age],B130,[1]!Table3[Film-Noir],1)</f>
         <v>3163</v>
       </c>
     </row>
@@ -2559,22 +2379,20 @@
         <v>16</v>
       </c>
       <c r="D131">
-        <f>COUNTIFS([1]!Table3[Gender],A131,[1]!Table3[Age],B131,[1]!Table3[Horror],1)</f>
         <v>3163</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B132" s="3">
+      <c r="A132" t="s">
+        <v>6</v>
+      </c>
+      <c r="B132">
         <v>1</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D132">
-        <f>COUNTIFS([1]!Table3[Gender],A132,[1]!Table3[Age],B132,[1]!Table3[Sci-Fi],1)</f>
         <v>3232</v>
       </c>
     </row>
@@ -2589,22 +2407,20 @@
         <v>11</v>
       </c>
       <c r="D133">
-        <f>COUNTIFS([1]!Table3[Gender],A133,[1]!Table3[Age],B133,[1]!Table3[Crime],1)</f>
         <v>3425</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B134" s="3">
+      <c r="A134" t="s">
+        <v>4</v>
+      </c>
+      <c r="B134">
         <v>25</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D134">
-        <f>COUNTIFS([1]!Table3[Gender],A134,[1]!Table3[Age],B134,[1]!Table3[Mystery],1)</f>
         <v>3485</v>
       </c>
     </row>
@@ -2615,11 +2431,10 @@
       <c r="B135">
         <v>56</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D135">
-        <f>COUNTIFS([1]!Table3[Gender],A135,[1]!Table3[Age],B135,[1]!Table3[Adventure],1)</f>
         <v>3680</v>
       </c>
     </row>
@@ -2630,56 +2445,52 @@
       <c r="B136">
         <v>45</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D136">
-        <f>COUNTIFS([1]!Table3[Gender],A136,[1]!Table3[Age],B136,[1]!Table3[Children''s],1)</f>
         <v>3696</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B137" s="3">
+      <c r="A137" t="s">
+        <v>6</v>
+      </c>
+      <c r="B137">
         <v>1</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D137">
-        <f>COUNTIFS([1]!Table3[Gender],A137,[1]!Table3[Age],B137,[1]!Table3[Thriller],1)</f>
         <v>3712</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B138" s="3">
+      <c r="A138" t="s">
+        <v>6</v>
+      </c>
+      <c r="B138">
         <v>35</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D138">
-        <f>COUNTIFS([1]!Table3[Gender],A138,[1]!Table3[Age],B138,[1]!Table3[Western],1)</f>
         <v>3755</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B139" s="3">
+      <c r="A139" t="s">
+        <v>4</v>
+      </c>
+      <c r="B139">
         <v>50</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D139">
-        <f>COUNTIFS([1]!Table3[Gender],A139,[1]!Table3[Age],B139,[1]!Table3[Romance],1)</f>
         <v>3783</v>
       </c>
     </row>
@@ -2690,11 +2501,10 @@
       <c r="B140">
         <v>25</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D140">
-        <f>COUNTIFS([1]!Table3[Gender],A140,[1]!Table3[Age],B140,[1]!Table3[Animation],1)</f>
         <v>3847</v>
       </c>
     </row>
@@ -2709,7 +2519,6 @@
         <v>10</v>
       </c>
       <c r="D141">
-        <f>COUNTIFS([1]!Table3[Gender],A141,[1]!Table3[Age],B141,[1]!Table3[Comedy],1)</f>
         <v>3860</v>
       </c>
     </row>
@@ -2724,37 +2533,34 @@
         <v>16</v>
       </c>
       <c r="D142">
-        <f>COUNTIFS([1]!Table3[Gender],A142,[1]!Table3[Age],B142,[1]!Table3[Horror],1)</f>
         <v>3953</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B143" s="3">
+      <c r="A143" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143">
         <v>45</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D143">
-        <f>COUNTIFS([1]!Table3[Gender],A143,[1]!Table3[Age],B143,[1]!Table3[Thriller],1)</f>
         <v>3975</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B144" s="3">
+      <c r="A144" t="s">
+        <v>6</v>
+      </c>
+      <c r="B144">
         <v>56</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D144">
-        <f>COUNTIFS([1]!Table3[Gender],A144,[1]!Table3[Age],B144,[1]!Table3[Sci-Fi],1)</f>
         <v>4073</v>
       </c>
     </row>
@@ -2769,37 +2575,34 @@
         <v>11</v>
       </c>
       <c r="D145">
-        <f>COUNTIFS([1]!Table3[Gender],A145,[1]!Table3[Age],B145,[1]!Table3[Crime],1)</f>
         <v>4235</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A146" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B146" s="3">
+      <c r="A146" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146">
         <v>56</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D146">
-        <f>COUNTIFS([1]!Table3[Gender],A146,[1]!Table3[Age],B146,[1]!Table3[Romance],1)</f>
         <v>4248</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A147" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B147" s="3">
+      <c r="A147" t="s">
+        <v>4</v>
+      </c>
+      <c r="B147">
         <v>25</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D147">
-        <f>COUNTIFS([1]!Table3[Gender],A147,[1]!Table3[Age],B147,[1]!Table3[Musical],1)</f>
         <v>4300</v>
       </c>
     </row>
@@ -2810,11 +2613,10 @@
       <c r="B148">
         <v>35</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D148">
-        <f>COUNTIFS([1]!Table3[Gender],A148,[1]!Table3[Age],B148,[1]!Table3[Children''s],1)</f>
         <v>4305</v>
       </c>
     </row>
@@ -2829,7 +2631,6 @@
         <v>11</v>
       </c>
       <c r="D149">
-        <f>COUNTIFS([1]!Table3[Gender],A149,[1]!Table3[Age],B149,[1]!Table3[Crime],1)</f>
         <v>4447</v>
       </c>
     </row>
@@ -2840,26 +2641,24 @@
       <c r="B150">
         <v>45</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D150">
-        <f>COUNTIFS([1]!Table3[Gender],A150,[1]!Table3[Age],B150,[1]!Table3[Action],1)</f>
         <v>4608</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A151" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B151" s="3">
+      <c r="A151" t="s">
+        <v>4</v>
+      </c>
+      <c r="B151">
         <v>25</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D151">
-        <f>COUNTIFS([1]!Table3[Gender],A151,[1]!Table3[Age],B151,[1]!Table3[War],1)</f>
         <v>4661</v>
       </c>
     </row>
@@ -2874,7 +2673,6 @@
         <v>13</v>
       </c>
       <c r="D152">
-        <f>COUNTIFS([1]!Table3[Gender],A152,[1]!Table3[Age],B152,[1]!Table3[Drama],1)</f>
         <v>4690</v>
       </c>
     </row>
@@ -2889,52 +2687,48 @@
         <v>13</v>
       </c>
       <c r="D153">
-        <f>COUNTIFS([1]!Table3[Gender],A153,[1]!Table3[Age],B153,[1]!Table3[Drama],1)</f>
         <v>4812</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A154" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B154" s="3">
+      <c r="A154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B154">
         <v>18</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D154">
-        <f>COUNTIFS([1]!Table3[Gender],A154,[1]!Table3[Age],B154,[1]!Table3[Musical],1)</f>
         <v>4820</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A155" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B155" s="3">
+      <c r="A155" t="s">
+        <v>4</v>
+      </c>
+      <c r="B155">
         <v>45</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D155">
-        <f>COUNTIFS([1]!Table3[Gender],A155,[1]!Table3[Age],B155,[1]!Table3[Romance],1)</f>
         <v>4863</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>6</v>
-      </c>
-      <c r="B156">
+      <c r="A156" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B156" s="3">
         <v>45</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D156">
-        <f>COUNTIFS([1]!Table3[Gender],A156,[1]!Table3[Age],B156,[1]!Table3[Horror],1)</f>
         <v>4873</v>
       </c>
     </row>
@@ -2949,7 +2743,6 @@
         <v>20</v>
       </c>
       <c r="D157">
-        <f>COUNTIFS([1]!Table3[Gender],A157,[1]!Table3[Age],B157,[1]!Table3[Sci-Fi],1)</f>
         <v>4928</v>
       </c>
     </row>
@@ -2964,7 +2757,6 @@
         <v>18</v>
       </c>
       <c r="D158">
-        <f>COUNTIFS([1]!Table3[Gender],A158,[1]!Table3[Age],B158,[1]!Table3[Mystery],1)</f>
         <v>4934</v>
       </c>
     </row>
@@ -2979,7 +2771,6 @@
         <v>22</v>
       </c>
       <c r="D159">
-        <f>COUNTIFS([1]!Table3[Gender],A159,[1]!Table3[Age],B159,[1]!Table3[War],1)</f>
         <v>4967</v>
       </c>
     </row>
@@ -2994,67 +2785,62 @@
         <v>22</v>
       </c>
       <c r="D160">
-        <f>COUNTIFS([1]!Table3[Gender],A160,[1]!Table3[Age],B160,[1]!Table3[War],1)</f>
         <v>5034</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>6</v>
-      </c>
-      <c r="B161">
+      <c r="A161" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B161" s="3">
         <v>25</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D161">
-        <f>COUNTIFS([1]!Table3[Gender],A161,[1]!Table3[Age],B161,[1]!Table3[Film-Noir],1)</f>
         <v>5165</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>4</v>
-      </c>
-      <c r="B162">
-        <v>18</v>
-      </c>
-      <c r="C162" t="s">
+      <c r="A162" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B162" s="3">
+        <v>18</v>
+      </c>
+      <c r="C162" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D162">
-        <f>COUNTIFS([1]!Table3[Gender],A162,[1]!Table3[Age],B162,[1]!Table3[Children''s],1)</f>
         <v>5234</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>6</v>
-      </c>
-      <c r="B163">
+      <c r="A163" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B163" s="3">
         <v>35</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D163">
-        <f>COUNTIFS([1]!Table3[Gender],A163,[1]!Table3[Age],B163,[1]!Table3[Fantasy],1)</f>
         <v>5234</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>6</v>
-      </c>
-      <c r="B164">
+      <c r="A164" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B164" s="3">
         <v>1</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D164">
-        <f>COUNTIFS([1]!Table3[Gender],A164,[1]!Table3[Age],B164,[1]!Table3[Action],1)</f>
         <v>5235</v>
       </c>
     </row>
@@ -3069,82 +2855,76 @@
         <v>21</v>
       </c>
       <c r="D165">
-        <f>COUNTIFS([1]!Table3[Gender],A165,[1]!Table3[Age],B165,[1]!Table3[Thriller],1)</f>
         <v>5291</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>4</v>
-      </c>
-      <c r="B166">
+      <c r="A166" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B166" s="3">
         <v>25</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D166">
-        <f>COUNTIFS([1]!Table3[Gender],A166,[1]!Table3[Age],B166,[1]!Table3[Horror],1)</f>
         <v>5379</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>4</v>
-      </c>
-      <c r="B167">
-        <v>18</v>
-      </c>
-      <c r="C167" t="s">
+      <c r="A167" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B167" s="3">
+        <v>18</v>
+      </c>
+      <c r="C167" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D167">
-        <f>COUNTIFS([1]!Table3[Gender],A167,[1]!Table3[Age],B167,[1]!Table3[Adventure],1)</f>
         <v>5430</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>6</v>
-      </c>
-      <c r="B168">
+      <c r="A168" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B168" s="3">
         <v>35</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C168" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D168">
-        <f>COUNTIFS([1]!Table3[Gender],A168,[1]!Table3[Age],B168,[1]!Table3[Animation],1)</f>
         <v>5718</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>4</v>
-      </c>
-      <c r="B169">
+      <c r="A169" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B169" s="3">
         <v>35</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D169">
-        <f>COUNTIFS([1]!Table3[Gender],A169,[1]!Table3[Age],B169,[1]!Table3[Adventure],1)</f>
         <v>5865</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>6</v>
-      </c>
-      <c r="B170">
+      <c r="A170" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B170" s="3">
         <v>18</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D170">
-        <f>COUNTIFS([1]!Table3[Gender],A170,[1]!Table3[Age],B170,[1]!Table3[Fantasy],1)</f>
         <v>5941</v>
       </c>
     </row>
@@ -3159,7 +2939,6 @@
         <v>18</v>
       </c>
       <c r="D171">
-        <f>COUNTIFS([1]!Table3[Gender],A171,[1]!Table3[Age],B171,[1]!Table3[Mystery],1)</f>
         <v>5987</v>
       </c>
     </row>
@@ -3174,7 +2953,6 @@
         <v>20</v>
       </c>
       <c r="D172">
-        <f>COUNTIFS([1]!Table3[Gender],A172,[1]!Table3[Age],B172,[1]!Table3[Sci-Fi],1)</f>
         <v>6009</v>
       </c>
     </row>
@@ -3189,7 +2967,6 @@
         <v>23</v>
       </c>
       <c r="D173">
-        <f>COUNTIFS([1]!Table3[Gender],A173,[1]!Table3[Age],B173,[1]!Table3[Western],1)</f>
         <v>6019</v>
       </c>
     </row>
@@ -3204,82 +2981,76 @@
         <v>17</v>
       </c>
       <c r="D174">
-        <f>COUNTIFS([1]!Table3[Gender],A174,[1]!Table3[Age],B174,[1]!Table3[Musical],1)</f>
         <v>6078</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>4</v>
-      </c>
-      <c r="B175">
+      <c r="A175" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B175" s="3">
         <v>25</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D175">
-        <f>COUNTIFS([1]!Table3[Gender],A175,[1]!Table3[Age],B175,[1]!Table3[Crime],1)</f>
         <v>6310</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>4</v>
-      </c>
-      <c r="B176">
+      <c r="A176" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B176" s="3">
         <v>50</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D176">
-        <f>COUNTIFS([1]!Table3[Gender],A176,[1]!Table3[Age],B176,[1]!Table3[Comedy],1)</f>
         <v>6399</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>4</v>
-      </c>
-      <c r="B177">
+      <c r="A177" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B177" s="3">
         <v>25</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D177">
-        <f>COUNTIFS([1]!Table3[Gender],A177,[1]!Table3[Age],B177,[1]!Table3[Children''s],1)</f>
         <v>6417</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>6</v>
-      </c>
-      <c r="B178">
+      <c r="A178" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B178" s="3">
         <v>56</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D178">
-        <f>COUNTIFS([1]!Table3[Gender],A178,[1]!Table3[Age],B178,[1]!Table3[Action],1)</f>
         <v>6883</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>6</v>
-      </c>
-      <c r="B179">
-        <v>18</v>
-      </c>
-      <c r="C179" t="s">
+      <c r="A179" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B179" s="3">
+        <v>18</v>
+      </c>
+      <c r="C179" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D179">
-        <f>COUNTIFS([1]!Table3[Gender],A179,[1]!Table3[Age],B179,[1]!Table3[Animation],1)</f>
         <v>7160</v>
       </c>
     </row>
@@ -3294,37 +3065,34 @@
         <v>21</v>
       </c>
       <c r="D180">
-        <f>COUNTIFS([1]!Table3[Gender],A180,[1]!Table3[Age],B180,[1]!Table3[Thriller],1)</f>
         <v>7290</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>6</v>
-      </c>
-      <c r="B181">
+      <c r="A181" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B181" s="3">
         <v>1</v>
       </c>
       <c r="C181" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D181">
-        <f>COUNTIFS([1]!Table3[Gender],A181,[1]!Table3[Age],B181,[1]!Table3[Comedy],1)</f>
         <v>7302</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>6</v>
-      </c>
-      <c r="B182">
+      <c r="A182" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B182" s="3">
         <v>50</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D182">
-        <f>COUNTIFS([1]!Table3[Gender],A182,[1]!Table3[Age],B182,[1]!Table3[Adventure],1)</f>
         <v>7336</v>
       </c>
     </row>
@@ -3339,37 +3107,34 @@
         <v>19</v>
       </c>
       <c r="D183">
-        <f>COUNTIFS([1]!Table3[Gender],A183,[1]!Table3[Age],B183,[1]!Table3[Romance],1)</f>
         <v>7590</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
-        <v>6</v>
-      </c>
-      <c r="B184">
+      <c r="A184" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B184" s="3">
         <v>45</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D184">
-        <f>COUNTIFS([1]!Table3[Gender],A184,[1]!Table3[Age],B184,[1]!Table3[Adventure],1)</f>
         <v>8090</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A185" t="s">
-        <v>4</v>
-      </c>
-      <c r="B185">
+      <c r="A185" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B185" s="3">
         <v>50</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D185">
-        <f>COUNTIFS([1]!Table3[Gender],A185,[1]!Table3[Age],B185,[1]!Table3[Drama],1)</f>
         <v>8237</v>
       </c>
     </row>
@@ -3384,22 +3149,20 @@
         <v>19</v>
       </c>
       <c r="D186">
-        <f>COUNTIFS([1]!Table3[Gender],A186,[1]!Table3[Age],B186,[1]!Table3[Romance],1)</f>
         <v>8420</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>4</v>
-      </c>
-      <c r="B187">
+      <c r="A187" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B187" s="3">
         <v>45</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D187">
-        <f>COUNTIFS([1]!Table3[Gender],A187,[1]!Table3[Age],B187,[1]!Table3[Comedy],1)</f>
         <v>8481</v>
       </c>
     </row>
@@ -3414,22 +3177,20 @@
         <v>21</v>
       </c>
       <c r="D188">
-        <f>COUNTIFS([1]!Table3[Gender],A188,[1]!Table3[Age],B188,[1]!Table3[Thriller],1)</f>
         <v>8560</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
-        <v>4</v>
-      </c>
-      <c r="B189">
-        <v>18</v>
-      </c>
-      <c r="C189" t="s">
+      <c r="A189" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B189" s="3">
+        <v>18</v>
+      </c>
+      <c r="C189" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D189">
-        <f>COUNTIFS([1]!Table3[Gender],A189,[1]!Table3[Age],B189,[1]!Table3[Action],1)</f>
         <v>8593</v>
       </c>
     </row>
@@ -3444,7 +3205,6 @@
         <v>22</v>
       </c>
       <c r="D190">
-        <f>COUNTIFS([1]!Table3[Gender],A190,[1]!Table3[Age],B190,[1]!Table3[War],1)</f>
         <v>8670</v>
       </c>
     </row>
@@ -3459,22 +3219,20 @@
         <v>20</v>
       </c>
       <c r="D191">
-        <f>COUNTIFS([1]!Table3[Gender],A191,[1]!Table3[Age],B191,[1]!Table3[Sci-Fi],1)</f>
         <v>8868</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
-        <v>6</v>
-      </c>
-      <c r="B192">
+      <c r="A192" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B192" s="3">
         <v>56</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D192">
-        <f>COUNTIFS([1]!Table3[Gender],A192,[1]!Table3[Age],B192,[1]!Table3[Comedy],1)</f>
         <v>8983</v>
       </c>
     </row>
@@ -3489,52 +3247,48 @@
         <v>19</v>
       </c>
       <c r="D193">
-        <f>COUNTIFS([1]!Table3[Gender],A193,[1]!Table3[Age],B193,[1]!Table3[Romance],1)</f>
         <v>9070</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
-        <v>4</v>
-      </c>
-      <c r="B194">
+      <c r="A194" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B194" s="3">
         <v>25</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C194" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D194">
-        <f>COUNTIFS([1]!Table3[Gender],A194,[1]!Table3[Age],B194,[1]!Table3[Adventure],1)</f>
         <v>9597</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
-        <v>6</v>
-      </c>
-      <c r="B195">
+      <c r="A195" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B195" s="3">
         <v>35</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D195">
-        <f>COUNTIFS([1]!Table3[Gender],A195,[1]!Table3[Age],B195,[1]!Table3[Children''s],1)</f>
         <v>9699</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
-        <v>4</v>
-      </c>
-      <c r="B196">
+      <c r="A196" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B196" s="3">
         <v>35</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C196" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D196">
-        <f>COUNTIFS([1]!Table3[Gender],A196,[1]!Table3[Age],B196,[1]!Table3[Action],1)</f>
         <v>9706</v>
       </c>
     </row>
@@ -3549,7 +3303,6 @@
         <v>19</v>
       </c>
       <c r="D197">
-        <f>COUNTIFS([1]!Table3[Gender],A197,[1]!Table3[Age],B197,[1]!Table3[Romance],1)</f>
         <v>9841</v>
       </c>
     </row>
@@ -3564,7 +3317,6 @@
         <v>20</v>
       </c>
       <c r="D198">
-        <f>COUNTIFS([1]!Table3[Gender],A198,[1]!Table3[Age],B198,[1]!Table3[Sci-Fi],1)</f>
         <v>10117</v>
       </c>
     </row>
@@ -3579,22 +3331,20 @@
         <v>20</v>
       </c>
       <c r="D199">
-        <f>COUNTIFS([1]!Table3[Gender],A199,[1]!Table3[Age],B199,[1]!Table3[Sci-Fi],1)</f>
         <v>10253</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
-        <v>4</v>
-      </c>
-      <c r="B200">
+      <c r="A200" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B200" s="3">
         <v>45</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D200">
-        <f>COUNTIFS([1]!Table3[Gender],A200,[1]!Table3[Age],B200,[1]!Table3[Drama],1)</f>
         <v>10287</v>
       </c>
     </row>
@@ -3609,7 +3359,6 @@
         <v>21</v>
       </c>
       <c r="D201">
-        <f>COUNTIFS([1]!Table3[Gender],A201,[1]!Table3[Age],B201,[1]!Table3[Thriller],1)</f>
         <v>10354</v>
       </c>
     </row>
@@ -3624,7 +3373,6 @@
         <v>17</v>
       </c>
       <c r="D202">
-        <f>COUNTIFS([1]!Table3[Gender],A202,[1]!Table3[Age],B202,[1]!Table3[Musical],1)</f>
         <v>10405</v>
       </c>
     </row>
@@ -3639,22 +3387,20 @@
         <v>21</v>
       </c>
       <c r="D203">
-        <f>COUNTIFS([1]!Table3[Gender],A203,[1]!Table3[Age],B203,[1]!Table3[Thriller],1)</f>
         <v>10958</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>6</v>
-      </c>
-      <c r="B204">
+      <c r="A204" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B204" s="3">
         <v>25</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D204">
-        <f>COUNTIFS([1]!Table3[Gender],A204,[1]!Table3[Age],B204,[1]!Table3[Fantasy],1)</f>
         <v>11266</v>
       </c>
     </row>
@@ -3669,22 +3415,20 @@
         <v>22</v>
       </c>
       <c r="D205">
-        <f>COUNTIFS([1]!Table3[Gender],A205,[1]!Table3[Age],B205,[1]!Table3[War],1)</f>
         <v>11417</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
-        <v>6</v>
-      </c>
-      <c r="B206">
+      <c r="A206" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B206" s="3">
         <v>35</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D206">
-        <f>COUNTIFS([1]!Table3[Gender],A206,[1]!Table3[Age],B206,[1]!Table3[Crime],1)</f>
         <v>11470</v>
       </c>
     </row>
@@ -3699,127 +3443,118 @@
         <v>18</v>
       </c>
       <c r="D207">
-        <f>COUNTIFS([1]!Table3[Gender],A207,[1]!Table3[Age],B207,[1]!Table3[Mystery],1)</f>
         <v>11675</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>6</v>
-      </c>
-      <c r="B208">
-        <v>18</v>
-      </c>
-      <c r="C208" t="s">
+      <c r="A208" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B208" s="3">
+        <v>18</v>
+      </c>
+      <c r="C208" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D208">
-        <f>COUNTIFS([1]!Table3[Gender],A208,[1]!Table3[Age],B208,[1]!Table3[Children''s],1)</f>
         <v>11690</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A209" t="s">
-        <v>6</v>
-      </c>
-      <c r="B209">
+      <c r="A209" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B209" s="3">
         <v>18</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D209">
-        <f>COUNTIFS([1]!Table3[Gender],A209,[1]!Table3[Age],B209,[1]!Table3[Horror],1)</f>
         <v>12021</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
-        <v>6</v>
-      </c>
-      <c r="B210">
+      <c r="A210" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B210" s="3">
         <v>35</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D210">
-        <f>COUNTIFS([1]!Table3[Gender],A210,[1]!Table3[Age],B210,[1]!Table3[Horror],1)</f>
         <v>12041</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A211" t="s">
-        <v>6</v>
-      </c>
-      <c r="B211">
+      <c r="A211" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B211" s="3">
         <v>18</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D211">
-        <f>COUNTIFS([1]!Table3[Gender],A211,[1]!Table3[Age],B211,[1]!Table3[Crime],1)</f>
         <v>12498</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
-        <v>6</v>
-      </c>
-      <c r="B212">
+      <c r="A212" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B212" s="3">
         <v>56</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D212">
-        <f>COUNTIFS([1]!Table3[Gender],A212,[1]!Table3[Age],B212,[1]!Table3[Drama],1)</f>
         <v>12579</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>6</v>
-      </c>
-      <c r="B213">
+      <c r="A213" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B213" s="3">
         <v>25</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C213" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D213">
-        <f>COUNTIFS([1]!Table3[Gender],A213,[1]!Table3[Age],B213,[1]!Table3[Animation],1)</f>
         <v>12607</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>6</v>
-      </c>
-      <c r="B214">
+      <c r="A214" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B214" s="3">
         <v>45</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C214" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D214">
-        <f>COUNTIFS([1]!Table3[Gender],A214,[1]!Table3[Age],B214,[1]!Table3[Action],1)</f>
         <v>14749</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
-        <v>6</v>
-      </c>
-      <c r="B215">
+      <c r="A215" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B215" s="3">
         <v>45</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C215" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D215">
-        <f>COUNTIFS([1]!Table3[Gender],A215,[1]!Table3[Age],B215,[1]!Table3[Action],1)</f>
         <v>14749</v>
       </c>
     </row>
@@ -3834,22 +3569,20 @@
         <v>21</v>
       </c>
       <c r="D216">
-        <f>COUNTIFS([1]!Table3[Gender],A216,[1]!Table3[Age],B216,[1]!Table3[Thriller],1)</f>
         <v>15239</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A217" t="s">
-        <v>4</v>
-      </c>
-      <c r="B217">
+      <c r="A217" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B217" s="3">
         <v>18</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D217">
-        <f>COUNTIFS([1]!Table3[Gender],A217,[1]!Table3[Age],B217,[1]!Table3[Drama],1)</f>
         <v>15977</v>
       </c>
     </row>
@@ -3864,52 +3597,48 @@
         <v>19</v>
       </c>
       <c r="D218">
-        <f>COUNTIFS([1]!Table3[Gender],A218,[1]!Table3[Age],B218,[1]!Table3[Romance],1)</f>
         <v>16586</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
-        <v>6</v>
-      </c>
-      <c r="B219">
+      <c r="A219" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B219" s="3">
         <v>50</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D219">
-        <f>COUNTIFS([1]!Table3[Gender],A219,[1]!Table3[Age],B219,[1]!Table3[Comedy],1)</f>
         <v>16734</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
-        <v>4</v>
-      </c>
-      <c r="B220">
+      <c r="A220" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B220" s="3">
         <v>25</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C220" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D220">
-        <f>COUNTIFS([1]!Table3[Gender],A220,[1]!Table3[Age],B220,[1]!Table3[Action],1)</f>
         <v>17147</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A221" t="s">
-        <v>4</v>
-      </c>
-      <c r="B221">
+      <c r="A221" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B221" s="3">
         <v>35</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D221">
-        <f>COUNTIFS([1]!Table3[Gender],A221,[1]!Table3[Age],B221,[1]!Table3[Comedy],1)</f>
         <v>18534</v>
       </c>
     </row>
@@ -3924,67 +3653,62 @@
         <v>19</v>
       </c>
       <c r="D222">
-        <f>COUNTIFS([1]!Table3[Gender],A222,[1]!Table3[Age],B222,[1]!Table3[Romance],1)</f>
         <v>19072</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A223" t="s">
-        <v>4</v>
-      </c>
-      <c r="B223">
+      <c r="A223" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B223" s="3">
         <v>18</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D223">
-        <f>COUNTIFS([1]!Table3[Gender],A223,[1]!Table3[Age],B223,[1]!Table3[Comedy],1)</f>
         <v>19136</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A224" t="s">
-        <v>4</v>
-      </c>
-      <c r="B224">
+      <c r="A224" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B224" s="3">
         <v>35</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D224">
-        <f>COUNTIFS([1]!Table3[Gender],A224,[1]!Table3[Age],B224,[1]!Table3[Drama],1)</f>
         <v>19239</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A225" t="s">
-        <v>6</v>
-      </c>
-      <c r="B225">
+      <c r="A225" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B225" s="3">
         <v>25</v>
       </c>
-      <c r="C225" t="s">
+      <c r="C225" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D225">
-        <f>COUNTIFS([1]!Table3[Gender],A225,[1]!Table3[Age],B225,[1]!Table3[Children''s],1)</f>
         <v>19326</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A226" t="s">
-        <v>6</v>
-      </c>
-      <c r="B226">
+      <c r="A226" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B226" s="3">
         <v>45</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D226">
-        <f>COUNTIFS([1]!Table3[Gender],A226,[1]!Table3[Age],B226,[1]!Table3[Comedy],1)</f>
         <v>19409</v>
       </c>
     </row>
@@ -3999,7 +3723,6 @@
         <v>19</v>
       </c>
       <c r="D227">
-        <f>COUNTIFS([1]!Table3[Gender],A227,[1]!Table3[Age],B227,[1]!Table3[Romance],1)</f>
         <v>19489</v>
       </c>
     </row>
@@ -4014,67 +3737,62 @@
         <v>22</v>
       </c>
       <c r="D228">
-        <f>COUNTIFS([1]!Table3[Gender],A228,[1]!Table3[Age],B228,[1]!Table3[War],1)</f>
         <v>20169</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A229" t="s">
-        <v>6</v>
-      </c>
-      <c r="B229">
+      <c r="A229" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B229" s="3">
         <v>35</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C229" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D229">
-        <f>COUNTIFS([1]!Table3[Gender],A229,[1]!Table3[Age],B229,[1]!Table3[Adventure],1)</f>
         <v>20817</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A230" t="s">
-        <v>6</v>
-      </c>
-      <c r="B230">
-        <v>18</v>
-      </c>
-      <c r="C230" t="s">
+      <c r="A230" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B230" s="3">
+        <v>18</v>
+      </c>
+      <c r="C230" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D230">
-        <f>COUNTIFS([1]!Table3[Gender],A230,[1]!Table3[Age],B230,[1]!Table3[Adventure],1)</f>
         <v>20894</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A231" t="s">
-        <v>6</v>
-      </c>
-      <c r="B231">
+      <c r="A231" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B231" s="3">
         <v>50</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D231">
-        <f>COUNTIFS([1]!Table3[Gender],A231,[1]!Table3[Age],B231,[1]!Table3[Drama],1)</f>
         <v>21010</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A232" t="s">
-        <v>6</v>
-      </c>
-      <c r="B232">
+      <c r="A232" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B232" s="3">
         <v>45</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D232">
-        <f>COUNTIFS([1]!Table3[Gender],A232,[1]!Table3[Age],B232,[1]!Table3[Drama],1)</f>
         <v>21854</v>
       </c>
     </row>
@@ -4089,22 +3807,20 @@
         <v>20</v>
       </c>
       <c r="D233">
-        <f>COUNTIFS([1]!Table3[Gender],A233,[1]!Table3[Age],B233,[1]!Table3[Sci-Fi],1)</f>
         <v>24105</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A234" t="s">
-        <v>6</v>
-      </c>
-      <c r="B234">
+      <c r="A234" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B234" s="3">
         <v>25</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D234">
-        <f>COUNTIFS([1]!Table3[Gender],A234,[1]!Table3[Age],B234,[1]!Table3[Horror],1)</f>
         <v>25856</v>
       </c>
     </row>
@@ -4119,22 +3835,20 @@
         <v>20</v>
       </c>
       <c r="D235">
-        <f>COUNTIFS([1]!Table3[Gender],A235,[1]!Table3[Age],B235,[1]!Table3[Sci-Fi],1)</f>
         <v>26324</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" t="s">
-        <v>6</v>
-      </c>
-      <c r="B236">
+      <c r="A236" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B236" s="3">
         <v>25</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D236">
-        <f>COUNTIFS([1]!Table3[Gender],A236,[1]!Table3[Age],B236,[1]!Table3[Crime],1)</f>
         <v>26720</v>
       </c>
     </row>
@@ -4149,7 +3863,6 @@
         <v>21</v>
       </c>
       <c r="D237">
-        <f>COUNTIFS([1]!Table3[Gender],A237,[1]!Table3[Age],B237,[1]!Table3[Thriller],1)</f>
         <v>28280</v>
       </c>
     </row>
@@ -4164,37 +3877,34 @@
         <v>21</v>
       </c>
       <c r="D238">
-        <f>COUNTIFS([1]!Table3[Gender],A238,[1]!Table3[Age],B238,[1]!Table3[Thriller],1)</f>
         <v>28587</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" t="s">
-        <v>4</v>
-      </c>
-      <c r="B239">
+      <c r="A239" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B239" s="3">
         <v>25</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D239">
-        <f>COUNTIFS([1]!Table3[Gender],A239,[1]!Table3[Age],B239,[1]!Table3[Comedy],1)</f>
         <v>36883</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A240" t="s">
-        <v>4</v>
-      </c>
-      <c r="B240">
+      <c r="A240" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B240" s="3">
         <v>25</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D240">
-        <f>COUNTIFS([1]!Table3[Gender],A240,[1]!Table3[Age],B240,[1]!Table3[Drama],1)</f>
         <v>37052</v>
       </c>
     </row>
@@ -4209,112 +3919,104 @@
         <v>19</v>
       </c>
       <c r="D241">
-        <f>COUNTIFS([1]!Table3[Gender],A241,[1]!Table3[Age],B241,[1]!Table3[Romance],1)</f>
         <v>38931</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A242" t="s">
-        <v>6</v>
-      </c>
-      <c r="B242">
+      <c r="A242" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B242" s="3">
         <v>35</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C242" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D242">
-        <f>COUNTIFS([1]!Table3[Gender],A242,[1]!Table3[Age],B242,[1]!Table3[Action],1)</f>
         <v>40797</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A243" t="s">
-        <v>6</v>
-      </c>
-      <c r="B243">
-        <v>18</v>
-      </c>
-      <c r="C243" t="s">
+      <c r="A243" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B243" s="3">
+        <v>18</v>
+      </c>
+      <c r="C243" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D243">
-        <f>COUNTIFS([1]!Table3[Gender],A243,[1]!Table3[Age],B243,[1]!Table3[Action],1)</f>
         <v>41593</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A244" t="s">
-        <v>6</v>
-      </c>
-      <c r="B244">
+      <c r="A244" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B244" s="3">
         <v>18</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D244">
-        <f>COUNTIFS([1]!Table3[Gender],A244,[1]!Table3[Age],B244,[1]!Table3[Drama],1)</f>
         <v>42127</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A245" t="s">
-        <v>6</v>
-      </c>
-      <c r="B245">
+      <c r="A245" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B245" s="3">
         <v>25</v>
       </c>
-      <c r="C245" t="s">
+      <c r="C245" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D245">
-        <f>COUNTIFS([1]!Table3[Gender],A245,[1]!Table3[Age],B245,[1]!Table3[Adventure],1)</f>
         <v>43036</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A246" t="s">
-        <v>6</v>
-      </c>
-      <c r="B246">
+      <c r="A246" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B246" s="3">
         <v>35</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D246">
-        <f>COUNTIFS([1]!Table3[Gender],A246,[1]!Table3[Age],B246,[1]!Table3[Comedy],1)</f>
         <v>50710</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A247" t="s">
-        <v>6</v>
-      </c>
-      <c r="B247">
+      <c r="A247" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B247" s="3">
         <v>18</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D247">
-        <f>COUNTIFS([1]!Table3[Gender],A247,[1]!Table3[Age],B247,[1]!Table3[Comedy],1)</f>
         <v>50844</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A248" t="s">
-        <v>6</v>
-      </c>
-      <c r="B248">
+      <c r="A248" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B248" s="3">
         <v>35</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D248">
-        <f>COUNTIFS([1]!Table3[Gender],A248,[1]!Table3[Age],B248,[1]!Table3[Drama],1)</f>
         <v>52351</v>
       </c>
     </row>
@@ -4329,7 +4031,6 @@
         <v>20</v>
       </c>
       <c r="D249">
-        <f>COUNTIFS([1]!Table3[Gender],A249,[1]!Table3[Age],B249,[1]!Table3[Sci-Fi],1)</f>
         <v>53039</v>
       </c>
     </row>
@@ -4344,59 +4045,52 @@
         <v>21</v>
       </c>
       <c r="D250">
-        <f>COUNTIFS([1]!Table3[Gender],A250,[1]!Table3[Age],B250,[1]!Table3[Thriller],1)</f>
         <v>62190</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A251" t="s">
-        <v>6</v>
-      </c>
-      <c r="B251">
+      <c r="A251" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B251" s="3">
         <v>25</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C251" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D251">
-        <f>COUNTIFS([1]!Table3[Gender],A251,[1]!Table3[Age],B251,[1]!Table3[Action],1)</f>
         <v>88531</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A252" t="s">
-        <v>6</v>
-      </c>
-      <c r="B252">
+      <c r="A252" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B252" s="3">
         <v>25</v>
       </c>
       <c r="C252" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D252">
-        <f>COUNTIFS([1]!Table3[Gender],A252,[1]!Table3[Age],B252,[1]!Table3[Drama],1)</f>
         <v>101643</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A253" t="s">
-        <v>6</v>
-      </c>
-      <c r="B253">
+      <c r="A253" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B253" s="3">
         <v>25</v>
       </c>
       <c r="C253" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D253">
-        <f>COUNTIFS([1]!Table3[Gender],A253,[1]!Table3[Age],B253,[1]!Table3[Comedy],1)</f>
         <v>106327</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>